<commit_message>
Include sourcing of packages in kobo_projectinit
</commit_message>
<xml_diff>
--- a/inst/script/XLSform_template.xlsx
+++ b/inst/script/XLSform_template.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="234">
   <si>
     <t>type</t>
   </si>
@@ -888,6 +888,77 @@
       <t xml:space="preserve">
   - 'ordinal': put TRUE if you want to keep the order as in the choices list. Otherwise, the data will be reorder by weighted frequency. Can be useful for likert questions (very satisfied, satisfied, etc.)</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The sampling_frame sheet allows you to put the information required to calculate your weights. The best option is to use this tool: https://oliviercecchi.shinyapps.io/R_sampling_tool_v2/
+You can then copy-paste the output into the sampling_frame sheet.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Make sure that the names of the columns where you input information are exactly as in the form.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> For example, if your strata are by district and displacement status, then the 'district' column should have the exact same spelling as in the 'choices'. Same goes for the displacement status.
+If you prefere to use your own sampling strategy, then make sure to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>keep the 'strata_pop'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">strata_pop </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>is where the actual population in this strata is stored (i.e. in the sampling_frame the first strata is IDP in Almar district).</t>
+    </r>
+  </si>
+  <si>
+    <t>appplies (all/rows)</t>
+  </si>
+  <si>
+    <t>all</t>
   </si>
   <si>
     <r>
@@ -1051,14 +1122,7 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">see 'survey' instructions' (Not implemented yet).
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The sampling_frame sheet allows you to put the information required to calculate your weights. The best option is to use this tool: https://oliviercecchi.shinyapps.io/R_sampling_tool_v2/
-You can then copy-paste the output into the sampling_frame sheet.
-</t>
+ - </t>
     </r>
     <r>
       <rPr>
@@ -1068,7 +1132,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Make sure that the names of the columns where you input information are exactly as in the form.</t>
+      <t>applies:</t>
     </r>
     <r>
       <rPr>
@@ -1077,18 +1141,17 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> For example, if your strata are by district and displacement status, then the 'district' column should have the exact same spelling as in the 'choices'. Same goes for the displacement status.
-If you prefere to use your own sampling strategy, then make sure to </t>
+      <t xml:space="preserve"> either "rows" or "all". Pick how you want to apply the calculation: </t>
     </r>
     <r>
       <rPr>
-        <b/>
+        <i/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>keep the 'strata_pop'</t>
+      <t>All:</t>
     </r>
     <r>
       <rPr>
@@ -1097,17 +1160,17 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">. </t>
+      <t xml:space="preserve"> calculation applies to all rows together (whole dataframe, but disaggregate if “disaggregation” is specified). </t>
     </r>
     <r>
       <rPr>
-        <b/>
+        <i/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">strata_pop </t>
+      <t>Rows:</t>
     </r>
     <r>
       <rPr>
@@ -1116,7 +1179,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>is where the actual population in this strata is stored (i.e. in the sampling_frame the first strata is IDP in Almar district).</t>
+      <t xml:space="preserve"> calculation applies to individual rows
+</t>
     </r>
   </si>
 </sst>
@@ -1124,13 +1188,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1279,6 +1349,13 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -1501,20 +1578,17 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1522,76 +1596,79 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -1599,68 +1676,72 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1669,7 +1750,27 @@
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2089,10 +2190,10 @@
   </sheetPr>
   <dimension ref="A1:T201"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G41" sqref="G41"/>
-      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3853,23 +3954,23 @@
   <sheetProtection algorithmName="SHA-512" hashValue="mSroYFNTr64/48FQ94JPx81+J7u+HC28/uZadpX6NOkkAePCLi9pKwYAp1V1iwFGmMFh4WEqhgw3eftX3m1UPg==" saltValue="gPemDYt/TeUTh7ASa4QTgw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <autoFilter ref="A1:T44"/>
   <conditionalFormatting sqref="B1 B46:B1048576">
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="autre">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="autre">
       <formula>NOT(ISERROR(SEARCH("autre",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="end_group">
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="end_group">
       <formula>NOT(ISERROR(SEARCH("end_group",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="begin_group">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="begin_group">
       <formula>NOT(ISERROR(SEARCH("begin_group",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="2058" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
@@ -7211,12 +7312,12 @@
     <sortCondition ref="C491"/>
   </sortState>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="autre">
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="autre">
       <formula>NOT(ISERROR(SEARCH("autre",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="2058" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
@@ -7275,7 +7376,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7286,10 +7387,11 @@
     <col min="4" max="4" width="35.85546875" style="31" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" style="31" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" style="31" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="31"/>
+    <col min="7" max="7" width="12.140625" style="31" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="27" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="27" customFormat="1" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>224</v>
       </c>
@@ -7308,7 +7410,9 @@
       <c r="F1" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="23"/>
+      <c r="G1" s="23" t="s">
+        <v>231</v>
+      </c>
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
@@ -7326,24 +7430,33 @@
       <c r="C2" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="42" t="s">
         <v>225</v>
       </c>
       <c r="E2" s="31" t="s">
         <v>61</v>
       </c>
+      <c r="F2" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>232</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="autre">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="autre">
       <formula>NOT(ISERROR(SEARCH("autre",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7634,12 +7747,12 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ygoPHPY0f9XEZGogRhWsi3vHK1DZP+f3BI3lyOT/jXoWcWYf92tVUnjqzV8g7ufx0A5WUCmFG9LVjFJlH5Cr+Q==" saltValue="Bi3tRPQZl1P9pCOLSDTPRg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="autre">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="autre">
       <formula>NOT(ISERROR(SEARCH("autre",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7653,148 +7766,148 @@
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="39"/>
-    <col min="4" max="4" width="81.42578125" style="39" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="39"/>
+    <col min="1" max="3" width="9.140625" style="38"/>
+    <col min="4" max="4" width="81.42578125" style="38" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="49" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="2" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="56" t="s">
         <v>216</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="42"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="46" t="s">
         <v>218</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="48"/>
     </row>
     <row r="5" spans="1:4" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="52"/>
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="53" t="s">
         <v>219</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="50"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="55"/>
     </row>
     <row r="7" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="50" t="s">
         <v>228</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="53"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="52"/>
     </row>
     <row r="8" spans="1:4" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="43" t="s">
         <v>220</v>
       </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="56"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="45"/>
     </row>
     <row r="9" spans="1:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="46" t="s">
         <v>221</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="47"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="48"/>
     </row>
     <row r="11" spans="1:4" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="43" t="s">
         <v>229</v>
       </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="56"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="46" t="s">
         <v>222</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="47"/>
-    </row>
-    <row r="13" spans="1:4" ht="162.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="54" t="s">
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="48"/>
+    </row>
+    <row r="13" spans="1:4" ht="216" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="45"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="48"/>
+    </row>
+    <row r="15" spans="1:4" ht="111.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="56"/>
-    </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
-        <v>226</v>
-      </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="47"/>
-    </row>
-    <row r="15" spans="1:4" ht="111.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="54" t="s">
-        <v>231</v>
-      </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="56"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A14:D14"/>
     <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>